<commit_message>
U resistive. Check the divider cable
</commit_message>
<xml_diff>
--- a/example/Shot_4/info.xlsx
+++ b/example/Shot_4/info.xlsx
@@ -8,17 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\uefe_waveform_interpreter\example\Shot_4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC5CD3D3-DA84-4EAD-9557-B38D99AE9BF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{395E1D5B-1B62-4636-B705-8D53EB5881E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -428,7 +437,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -626,7 +635,8 @@
         <v>26</v>
       </c>
       <c r="B18">
-        <v>910</v>
+        <f>1000/0.91</f>
+        <v>1098.901098901099</v>
       </c>
       <c r="C18" t="s">
         <v>11</v>

</xml_diff>